<commit_message>
Update V sin nombre de Archivos
</commit_message>
<xml_diff>
--- a/Categorias.xlsx
+++ b/Categorias.xlsx
@@ -5,27 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\Control-Monotributistas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Python\Scripts\Control-Monotributistas\LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4DAFC3-E519-4D46-9CEE-5A2BC30DD117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF200F4-2B5A-452C-825D-459ABBF15EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categoria" sheetId="1" r:id="rId1"/>
+    <sheet name="Rango de Fechas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -66,14 +78,20 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>Sin Categoria</t>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Fuera de Parámetros del monotributo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +115,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -112,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,11 +146,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -139,6 +180,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,13 +524,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -586,9 +630,9 @@
         <v>8040721.1900000004</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4">
         <v>9.9999999999999898E+18</v>
@@ -604,4 +648,37 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D29C3E0-2AFE-4375-A5EF-B205ADFDDEE0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>44743</v>
+      </c>
+      <c r="B2" s="7">
+        <f>EDATE(A2,12)-1</f>
+        <v>45107</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>